<commit_message>
Update template to latest working version
</commit_message>
<xml_diff>
--- a/sideload-template.xlsx
+++ b/sideload-template.xlsx
@@ -107,25 +107,25 @@
     <t>path</t>
   </si>
   <si>
+    <t>Sample Type</t>
+  </si>
+  <si>
+    <t>sample_type</t>
+  </si>
+  <si>
+    <t>Cell Type</t>
+  </si>
+  <si>
+    <t>cell_type</t>
+  </si>
+  <si>
     <t>Intrument</t>
   </si>
   <si>
-    <t>Sample Type</t>
-  </si>
-  <si>
-    <t>Cell Type</t>
+    <t>instrument</t>
   </si>
   <si>
     <t>Path to dta folder</t>
-  </si>
-  <si>
-    <t>instrument</t>
-  </si>
-  <si>
-    <t>sample_type</t>
-  </si>
-  <si>
-    <t>cell_type</t>
   </si>
 </sst>
 </file>
@@ -488,24 +488,34 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="S11" sqref="S11"/>
+      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.88671875" customWidth="1"/>
-    <col min="5" max="5" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="30" bestFit="1" customWidth="1"/>
-    <col min="15" max="23" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="14.88671875" customWidth="1"/>
+    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="17" customWidth="1"/>
+    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="33.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="35.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="27.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="83.5546875" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="85.109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="78" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="75" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="22" max="26" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
@@ -519,7 +529,7 @@
         <v>14</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>15</v>
@@ -528,7 +538,7 @@
         <v>16</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>29</v>
@@ -558,7 +568,7 @@
         <v>25</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="R1" s="1" t="str">
         <f>"Replicate " &amp;COLUMN()-COLUMN($Q$1) &amp; " path"</f>
@@ -612,7 +622,7 @@
         <v>2</v>
       </c>
       <c r="D2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="E2" t="s">
         <v>9</v>
@@ -621,10 +631,10 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="I2" t="s">
         <v>3</v>

</xml_diff>

<commit_message>
Update template and also save as csv for git
</commit_message>
<xml_diff>
--- a/sideload-template.xlsx
+++ b/sideload-template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17030"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
   <si>
     <t>name</t>
   </si>
@@ -35,33 +35,12 @@
     <t>experiment_type</t>
   </si>
   <si>
-    <t>probe</t>
-  </si>
-  <si>
-    <t>treatment_details.probe.concentration</t>
-  </si>
-  <si>
-    <t>treatment_details.probe.time</t>
-  </si>
-  <si>
-    <t>inhibitor</t>
-  </si>
-  <si>
-    <t>treatment_details.inhibitor.concentration</t>
-  </si>
-  <si>
-    <t>treatment_details.inhibitor.time</t>
-  </si>
-  <si>
     <t>treatment_type</t>
   </si>
   <si>
     <t>proteomic_fraction</t>
   </si>
   <si>
-    <t>treatment_details.inhibitor.treated_fraction</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -80,30 +59,9 @@
     <t>Probe</t>
   </si>
   <si>
-    <t>Probe Concentration</t>
-  </si>
-  <si>
-    <t>Probe Treatment Time</t>
-  </si>
-  <si>
     <t>Inhibitor</t>
   </si>
   <si>
-    <t>Inhibitor Concentration</t>
-  </si>
-  <si>
-    <t>Inhibitor Treatment Time</t>
-  </si>
-  <si>
-    <t>Treated Fraction (H/L/both/none)</t>
-  </si>
-  <si>
-    <t>ratio_numerator</t>
-  </si>
-  <si>
-    <t>Quantification Numerator</t>
-  </si>
-  <si>
     <t>path</t>
   </si>
   <si>
@@ -126,13 +84,110 @@
   </si>
   <si>
     <t>Path to dta folder</t>
+  </si>
+  <si>
+    <t>Probe Treatment Time (hours)</t>
+  </si>
+  <si>
+    <t>Inhibitor Treatment Time (hours)</t>
+  </si>
+  <si>
+    <t>Quantification Numerator (H/L)</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>Light Fraction</t>
+  </si>
+  <si>
+    <r>
+      <t>Inhibitor Concentration (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>µ</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="7.7"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>M)</t>
+    </r>
+  </si>
+  <si>
+    <t>Probe Concentration (µM)</t>
+  </si>
+  <si>
+    <t>Heavy Fraction</t>
+  </si>
+  <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t>date</t>
+  </si>
+  <si>
+    <t>Metadata</t>
+  </si>
+  <si>
+    <t>treament.Lt.inhibitor.name</t>
+  </si>
+  <si>
+    <t>treament.Lt.inhibitor.concentration</t>
+  </si>
+  <si>
+    <t>treament.Lt.inhibitor.time</t>
+  </si>
+  <si>
+    <t>treament.Lt.probe.name</t>
+  </si>
+  <si>
+    <t>treament.Lt.probe.concentration</t>
+  </si>
+  <si>
+    <t>treament.Lt.probe.time</t>
+  </si>
+  <si>
+    <t>treament.H.inhibitor.name</t>
+  </si>
+  <si>
+    <t>treament.H.inhibitor.concentration</t>
+  </si>
+  <si>
+    <t>treament.H.inhibitor.time</t>
+  </si>
+  <si>
+    <t>treament.H.probe.name</t>
+  </si>
+  <si>
+    <t>treament.H.probe.concentration</t>
+  </si>
+  <si>
+    <t>treament.H.probe.time</t>
+  </si>
+  <si>
+    <t>quantification_numerator</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -148,13 +203,39 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="7.7"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -169,9 +250,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -486,225 +582,303 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA2"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AH3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A15" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A30" sqref="A30"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="39.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="14.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="17" customWidth="1"/>
-    <col min="9" max="9" width="19.109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="33.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.5546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="18.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="35.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="27.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="30" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="83.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="85.109375" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="78" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="75" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="70.88671875" bestFit="1" customWidth="1"/>
-    <col min="22" max="26" width="14.88671875" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="34.88671875" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="14.77734375" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.5546875" customWidth="1"/>
+    <col min="7" max="7" width="15.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.5546875" customWidth="1"/>
+    <col min="9" max="9" width="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" customWidth="1"/>
+    <col min="11" max="11" width="16.21875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
+    <col min="13" max="23" width="20.77734375" customWidth="1"/>
+    <col min="24" max="24" width="83.5546875" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="85.109375" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="78" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="75" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="70.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="33" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" s="1" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:34" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
+      <c r="L1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
+      <c r="Q1" s="5"/>
+      <c r="R1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6"/>
+      <c r="W1" s="6"/>
+    </row>
+    <row r="2" spans="1:34" s="1" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="J2" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="K2" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="Q2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="R2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="W2" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="X2" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R1" s="1" t="str">
-        <f>"Replicate " &amp;COLUMN()-COLUMN($Q$1) &amp; " path"</f>
+      <c r="Y2" s="1" t="str">
+        <f>"Replicate " &amp;COLUMN()-COLUMN($X$2) &amp; " path"</f>
         <v>Replicate 1 path</v>
       </c>
-      <c r="S1" s="1" t="str">
-        <f>"Replicate " &amp;COLUMN()-COLUMN($Q$1) &amp; " path"</f>
+      <c r="Z2" s="1" t="str">
+        <f>"Replicate " &amp;COLUMN()-COLUMN($X$2) &amp; " path"</f>
         <v>Replicate 2 path</v>
       </c>
-      <c r="T1" s="1" t="str">
-        <f t="shared" ref="T1:AA1" si="0">"Replicate " &amp;COLUMN()-COLUMN($Q$1) &amp; " path"</f>
+      <c r="AA2" s="1" t="str">
+        <f t="shared" ref="AA2:AH2" si="0">"Replicate " &amp;COLUMN()-COLUMN($X$2) &amp; " path"</f>
         <v>Replicate 3 path</v>
       </c>
-      <c r="U1" s="1" t="str">
+      <c r="AB2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 4 path</v>
       </c>
-      <c r="V1" s="1" t="str">
+      <c r="AC2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 5 path</v>
       </c>
-      <c r="W1" s="1" t="str">
+      <c r="AD2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 6 path</v>
       </c>
-      <c r="X1" s="1" t="str">
+      <c r="AE2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 7 path</v>
       </c>
-      <c r="Y1" s="1" t="str">
+      <c r="AF2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 8 path</v>
       </c>
-      <c r="Z1" s="1" t="str">
+      <c r="AG2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 9 path</v>
       </c>
-      <c r="AA1" s="1" t="str">
+      <c r="AH2" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Replicate 10 path</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="3" spans="1:34" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" t="s">
         <v>1</v>
       </c>
-      <c r="C2" t="s">
+      <c r="E3" t="s">
         <v>2</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F3" t="s">
+        <v>18</v>
+      </c>
+      <c r="G3" t="s">
+        <v>3</v>
+      </c>
+      <c r="H3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J3" t="s">
+        <v>16</v>
+      </c>
+      <c r="K3" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" t="s">
         <v>32</v>
       </c>
-      <c r="E2" t="s">
-        <v>9</v>
-      </c>
-      <c r="F2" t="s">
-        <v>10</v>
-      </c>
-      <c r="G2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J2" t="s">
-        <v>4</v>
-      </c>
-      <c r="K2" t="s">
-        <v>5</v>
-      </c>
-      <c r="L2" t="s">
-        <v>6</v>
-      </c>
-      <c r="M2" t="s">
-        <v>7</v>
-      </c>
-      <c r="N2" t="s">
-        <v>8</v>
-      </c>
-      <c r="O2" t="s">
-        <v>11</v>
-      </c>
-      <c r="P2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>26</v>
-      </c>
-      <c r="R2" t="str">
-        <f>"replicate_" &amp;COLUMN()-COLUMN($Q$1) &amp; "_path"</f>
+      <c r="M3" t="s">
+        <v>33</v>
+      </c>
+      <c r="N3" t="s">
+        <v>34</v>
+      </c>
+      <c r="O3" t="s">
+        <v>35</v>
+      </c>
+      <c r="P3" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>37</v>
+      </c>
+      <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" t="s">
+        <v>40</v>
+      </c>
+      <c r="U3" t="s">
+        <v>41</v>
+      </c>
+      <c r="V3" t="s">
+        <v>42</v>
+      </c>
+      <c r="W3" t="s">
+        <v>43</v>
+      </c>
+      <c r="X3" t="s">
+        <v>12</v>
+      </c>
+      <c r="Y3" t="str">
+        <f>"replicate_" &amp;COLUMN()-COLUMN($X$2) &amp; "_path"</f>
         <v>replicate_1_path</v>
       </c>
-      <c r="S2" t="str">
-        <f t="shared" ref="S2:AA2" si="1">"replicate_" &amp;COLUMN()-COLUMN($Q$1) &amp; "_path"</f>
+      <c r="Z3" t="str">
+        <f t="shared" ref="Z3:AH3" si="1">"replicate_" &amp;COLUMN()-COLUMN($X$2) &amp; "_path"</f>
         <v>replicate_2_path</v>
       </c>
-      <c r="T2" t="str">
+      <c r="AA3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_3_path</v>
       </c>
-      <c r="U2" t="str">
+      <c r="AB3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_4_path</v>
       </c>
-      <c r="V2" t="str">
+      <c r="AC3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_5_path</v>
       </c>
-      <c r="W2" t="str">
+      <c r="AD3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_6_path</v>
       </c>
-      <c r="X2" t="str">
+      <c r="AE3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_7_path</v>
       </c>
-      <c r="Y2" t="str">
+      <c r="AF3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_8_path</v>
       </c>
-      <c r="Z2" t="str">
+      <c r="AG3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_9_path</v>
       </c>
-      <c r="AA2" t="str">
+      <c r="AH3" t="str">
         <f t="shared" si="1"/>
         <v>replicate_10_path</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="L1:Q1"/>
+    <mergeCell ref="R1:W1"/>
+    <mergeCell ref="A1:K1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Fixed spelling mistakes and added id suffixes where needed.
</commit_message>
<xml_diff>
--- a/sideload-template.xlsx
+++ b/sideload-template.xlsx
@@ -29,15 +29,6 @@
     <t>name</t>
   </si>
   <si>
-    <t>organism</t>
-  </si>
-  <si>
-    <t>experiment_type</t>
-  </si>
-  <si>
-    <t>proteomic_fraction</t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -62,19 +53,10 @@
     <t>Sample Type</t>
   </si>
   <si>
-    <t>sample_type</t>
-  </si>
-  <si>
     <t>Cell Type</t>
   </si>
   <si>
-    <t>cell_type</t>
-  </si>
-  <si>
     <t>Intrument</t>
-  </si>
-  <si>
-    <t>instrument</t>
   </si>
   <si>
     <t>Path to dta folder</t>
@@ -138,45 +120,9 @@
     <t>Metadata</t>
   </si>
   <si>
-    <t>treament.H.inhibitor.name</t>
-  </si>
-  <si>
-    <t>treament.H.inhibitor.concentration</t>
-  </si>
-  <si>
-    <t>treament.H.inhibitor.time</t>
-  </si>
-  <si>
-    <t>treament.H.probe.name</t>
-  </si>
-  <si>
-    <t>treament.H.probe.concentration</t>
-  </si>
-  <si>
-    <t>treament.H.probe.time</t>
-  </si>
-  <si>
     <t>quantification_numerator</t>
   </si>
   <si>
-    <t>treament.L.inhibitor.name</t>
-  </si>
-  <si>
-    <t>treament.L.inhibitor.concentration</t>
-  </si>
-  <si>
-    <t>treament.L.inhibitor.time</t>
-  </si>
-  <si>
-    <t>treament.L.probe.name</t>
-  </si>
-  <si>
-    <t>treament.L.probe.concentration</t>
-  </si>
-  <si>
-    <t>treament.L.probe.time</t>
-  </si>
-  <si>
     <t>Inhibitor Treatment Type (in situ etc.)</t>
   </si>
   <si>
@@ -193,6 +139,60 @@
   </si>
   <si>
     <t>treatment.H.inhibitor.method</t>
+  </si>
+  <si>
+    <t>organism_id</t>
+  </si>
+  <si>
+    <t>experiment_type_id</t>
+  </si>
+  <si>
+    <t>instrument_id</t>
+  </si>
+  <si>
+    <t>proteomic_fraction_id</t>
+  </si>
+  <si>
+    <t>sample_type_id</t>
+  </si>
+  <si>
+    <t>cell_type_id</t>
+  </si>
+  <si>
+    <t>treatment.L.inhibitor.time</t>
+  </si>
+  <si>
+    <t>treatment.L.probe.concentration</t>
+  </si>
+  <si>
+    <t>treatment.L.probe.id</t>
+  </si>
+  <si>
+    <t>treatment.L.probe.time</t>
+  </si>
+  <si>
+    <t>treatment.H.inhibitor.id</t>
+  </si>
+  <si>
+    <t>treatment.L.inhibitor.id</t>
+  </si>
+  <si>
+    <t>treatment.L.inhibitor.concentration</t>
+  </si>
+  <si>
+    <t>treatment.H.inhibitor.concentration</t>
+  </si>
+  <si>
+    <t>treatment.H.inhibitor.time</t>
+  </si>
+  <si>
+    <t>treatment.H.probe.concentration</t>
+  </si>
+  <si>
+    <t>treatment.H.probe.time</t>
+  </si>
+  <si>
+    <t>treatment.H.probe.id</t>
   </si>
 </sst>
 </file>
@@ -627,7 +627,7 @@
   <sheetData>
     <row r="1" spans="1:37" x14ac:dyDescent="0.3">
       <c r="A1" s="6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="B1" s="6"/>
       <c r="C1" s="6"/>
@@ -639,7 +639,7 @@
       <c r="I1" s="6"/>
       <c r="J1" s="6"/>
       <c r="K1" s="5" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="L1" s="5"/>
       <c r="M1" s="5"/>
@@ -649,7 +649,7 @@
       <c r="Q1" s="5"/>
       <c r="R1" s="5"/>
       <c r="S1" s="6" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="T1" s="6"/>
       <c r="U1" s="6"/>
@@ -661,85 +661,85 @@
     </row>
     <row r="2" spans="1:37" s="1" customFormat="1" ht="49.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="W2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="X2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="Y2" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA2" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="N2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="O2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Q2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="W2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="X2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="Y2" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="Z2" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="AA2" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="AB2" s="1" t="str">
         <f>"Replicate " &amp;COLUMN()-COLUMN($AA$2) &amp; " path"</f>
@@ -787,82 +787,82 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="D3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G3" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+      <c r="I3" t="s">
+        <v>36</v>
+      </c>
+      <c r="J3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" t="s">
+        <v>42</v>
+      </c>
+      <c r="L3" t="s">
+        <v>43</v>
+      </c>
+      <c r="M3" t="s">
+        <v>26</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" t="s">
+        <v>39</v>
+      </c>
+      <c r="P3" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>16</v>
-      </c>
-      <c r="G3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H3" t="s">
-        <v>12</v>
-      </c>
-      <c r="I3" t="s">
-        <v>14</v>
-      </c>
-      <c r="J3" t="s">
-        <v>36</v>
-      </c>
-      <c r="K3" t="s">
-        <v>37</v>
-      </c>
-      <c r="L3" t="s">
-        <v>38</v>
-      </c>
-      <c r="M3" t="s">
+      <c r="R3" t="s">
+        <v>40</v>
+      </c>
+      <c r="S3" t="s">
+        <v>41</v>
+      </c>
+      <c r="T3" t="s">
         <v>44</v>
       </c>
-      <c r="N3" t="s">
-        <v>39</v>
-      </c>
-      <c r="O3" t="s">
-        <v>40</v>
-      </c>
-      <c r="P3" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q3" t="s">
+      <c r="U3" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" t="s">
+        <v>45</v>
+      </c>
+      <c r="W3" t="s">
+        <v>48</v>
+      </c>
+      <c r="X3" t="s">
         <v>46</v>
       </c>
-      <c r="R3" t="s">
-        <v>42</v>
-      </c>
-      <c r="S3" t="s">
-        <v>30</v>
-      </c>
-      <c r="T3" t="s">
-        <v>31</v>
-      </c>
-      <c r="U3" t="s">
-        <v>48</v>
-      </c>
-      <c r="V3" t="s">
-        <v>32</v>
-      </c>
-      <c r="W3" t="s">
-        <v>33</v>
-      </c>
-      <c r="X3" t="s">
-        <v>34</v>
-      </c>
       <c r="Y3" t="s">
+        <v>29</v>
+      </c>
+      <c r="Z3" t="s">
         <v>47</v>
       </c>
-      <c r="Z3" t="s">
-        <v>35</v>
-      </c>
       <c r="AA3" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="AB3" t="str">
         <f>"replicate_" &amp;COLUMN()-COLUMN($AA$2) &amp; "_path"</f>

</xml_diff>